<commit_message>
report finalised I think
</commit_message>
<xml_diff>
--- a/iitbProc/control.xlsx
+++ b/iitbProc/control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\IITB\CS 226 DLD\Project\iitbProc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D23A1D0-9C19-4603-A17D-C9C260E798AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85EF1D8-8A1D-4039-B24A-935BDBD13B7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,35 +810,6 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1630,25 +1601,54 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1665,40 +1665,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9226B7C0-913C-476E-8E7F-82FC02DD7221}" name="Table5" displayName="Table5" ref="B3:AF25" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="33" tableBorderDxfId="34" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9226B7C0-913C-476E-8E7F-82FC02DD7221}" name="Table5" displayName="Table5" ref="B3:AF25" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="B3:AF25" xr:uid="{8035ED20-D866-4FCE-B281-F8347C417473}"/>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{27AA2535-A3B4-4B7D-95FE-BF45A3EB6224}" name="Column1" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{B6F07219-B3C0-44E9-B431-1660565DDCAD}" name="w1" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{4A494FEC-8678-4A8F-901B-C2895111DDD7}" name="w2" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{8925CE30-5D92-4A0A-B553-35C81767D723}" name="w3" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{9B1F7966-CC7F-46BF-B957-93C10DCFCE98}" name="w4" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{E0186CE6-587D-42EA-AB72-347C7F94307C}" name="w5" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{CB1B1C3F-69F6-4500-BBC1-2C01284C6815}" name="w6" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{C204D9B0-B248-44FB-B44B-42A98ABD9BD2}" name="w7" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{A32DC7E9-6E4F-4CD2-A6CD-9E7FF9906204}" name="m1" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{62E9AAE3-D62C-4F78-83FF-FB9AB134947E}" name="m12" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{71C1034D-20E9-4515-ABB8-D4B005D63D28}" name="m21" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{3A2356E5-AEBD-4226-98A2-1BD9B51A01D9}" name="m20" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{D2CC2E30-AB33-4365-99E7-20CA5846C394}" name="m31" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{A7B48B3E-AA53-41FE-B5A3-ED2341588EC8}" name="m30" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{8EE771DB-7681-4511-980C-CE64B93487E8}" name="m4" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{BC2FD657-66FE-42C0-9A0D-2FED55E6E832}" name="m51" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{AD47E79E-7240-4F09-86FE-CAD60E5D1B37}" name="m50" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{592E39A6-7FA5-4001-9F8F-E5B1D874F44D}" name="m61" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{C06EFA5E-1275-48AC-BC67-7959180378C5}" name="m60" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{22A678B7-BBEF-4C43-91C5-33CF1671E8D3}" name="m71" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{142E1F39-69B7-4A86-9743-4F3DBD141E7E}" name="m70" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{662F688B-BA4F-4DEA-B362-82526C268A91}" name="m8" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{7C21D2B7-892F-439D-A7B6-CE402E0B0B4A}" name="m92" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{5473C5FB-D67C-45EE-8477-927BA82692AF}" name="m91" dataDxfId="8"/>
-    <tableColumn id="25" xr3:uid="{F48E4D4D-7B32-494F-92B1-F0EB1C6F7338}" name="m90" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{2D480CB9-6CE4-4BD4-980D-2D3E75547E85}" name="m101" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{57951F71-035C-4210-A81C-0E90DF516832}" name="m100" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{E42BE5C4-6192-4901-BE4F-41D271CCFE46}" name="wc" dataDxfId="4"/>
-    <tableColumn id="29" xr3:uid="{1770861A-0AFA-40CA-B67C-FD2FD721CA47}" name="wz" dataDxfId="3"/>
-    <tableColumn id="30" xr3:uid="{ED3474C8-B1DF-454A-A982-B5CE54F098EE}" name="mz" dataDxfId="2"/>
-    <tableColumn id="31" xr3:uid="{D29BE6E9-ED4C-46D6-9B73-A205D7886628}" name="alu_op" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{27AA2535-A3B4-4B7D-95FE-BF45A3EB6224}" name="Column1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{B6F07219-B3C0-44E9-B431-1660565DDCAD}" name="w1" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{4A494FEC-8678-4A8F-901B-C2895111DDD7}" name="w2" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{8925CE30-5D92-4A0A-B553-35C81767D723}" name="w3" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{9B1F7966-CC7F-46BF-B957-93C10DCFCE98}" name="w4" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{E0186CE6-587D-42EA-AB72-347C7F94307C}" name="w5" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{CB1B1C3F-69F6-4500-BBC1-2C01284C6815}" name="w6" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{C204D9B0-B248-44FB-B44B-42A98ABD9BD2}" name="w7" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{A32DC7E9-6E4F-4CD2-A6CD-9E7FF9906204}" name="m1" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{62E9AAE3-D62C-4F78-83FF-FB9AB134947E}" name="m12" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{71C1034D-20E9-4515-ABB8-D4B005D63D28}" name="m21" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{3A2356E5-AEBD-4226-98A2-1BD9B51A01D9}" name="m20" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{D2CC2E30-AB33-4365-99E7-20CA5846C394}" name="m31" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{A7B48B3E-AA53-41FE-B5A3-ED2341588EC8}" name="m30" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{8EE771DB-7681-4511-980C-CE64B93487E8}" name="m4" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{BC2FD657-66FE-42C0-9A0D-2FED55E6E832}" name="m51" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{AD47E79E-7240-4F09-86FE-CAD60E5D1B37}" name="m50" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{592E39A6-7FA5-4001-9F8F-E5B1D874F44D}" name="m61" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{C06EFA5E-1275-48AC-BC67-7959180378C5}" name="m60" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{22A678B7-BBEF-4C43-91C5-33CF1671E8D3}" name="m71" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{142E1F39-69B7-4A86-9743-4F3DBD141E7E}" name="m70" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{662F688B-BA4F-4DEA-B362-82526C268A91}" name="m8" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{7C21D2B7-892F-439D-A7B6-CE402E0B0B4A}" name="m92" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{5473C5FB-D67C-45EE-8477-927BA82692AF}" name="m91" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{F48E4D4D-7B32-494F-92B1-F0EB1C6F7338}" name="m90" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{2D480CB9-6CE4-4BD4-980D-2D3E75547E85}" name="m101" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{57951F71-035C-4210-A81C-0E90DF516832}" name="m100" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{E42BE5C4-6192-4901-BE4F-41D271CCFE46}" name="wc" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{1770861A-0AFA-40CA-B67C-FD2FD721CA47}" name="wz" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{ED3474C8-B1DF-454A-A982-B5CE54F098EE}" name="mz" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{D29BE6E9-ED4C-46D6-9B73-A205D7886628}" name="alu_op" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3391,10 +3391,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD77549-DBC6-48CA-BA65-3A708FEF6E16}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B3:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4793,9 +4796,11 @@
       <c r="AB31" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>